<commit_message>
* Added the support for report type specific options. * Added 'autoFilter' excel option. * Added 'autoSize' excel option. * Added 'headerStyle' excel option. * Other minor cleanups.
</commit_message>
<xml_diff>
--- a/tests/data/desired/joinreport.xlsx
+++ b/tests/data/desired/joinreport.xlsx
@@ -1,37 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="full" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="left" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="right" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="inner" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="interlaced" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="diffs" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="full" r:id="rId3" sheetId="1"/>
+    <sheet name="left" r:id="rId4" sheetId="2"/>
+    <sheet name="right" r:id="rId5" sheetId="3"/>
+    <sheet name="inner" r:id="rId6" sheetId="4"/>
+    <sheet name="interlaced" r:id="rId7" sheetId="5"/>
+    <sheet name="diffs" r:id="rId8" sheetId="6"/>
     <sheet name="append" r:id="rId9" sheetId="7"/>
     <sheet name="multicols" r:id="rId10" sheetId="8"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="Excel_BuiltIn_Print_Area_1" vbProcedure="false"/>
-    <definedName function="false" hidden="false" name="Excel_BuiltIn_Sheet_Title_1" vbProcedure="false">"full"</definedName>
-    <definedName function="false" hidden="false" name="Excel_BuiltIn_Print_Area_2" vbProcedure="false"/>
-    <definedName function="false" hidden="false" name="Excel_BuiltIn_Sheet_Title_2" vbProcedure="false">"left"</definedName>
-    <definedName function="false" hidden="false" name="Excel_BuiltIn_Print_Area_3" vbProcedure="false"/>
-    <definedName function="false" hidden="false" name="Excel_BuiltIn_Sheet_Title_3" vbProcedure="false">"right"</definedName>
-    <definedName function="false" hidden="false" name="Excel_BuiltIn_Print_Area_4" vbProcedure="false"/>
-    <definedName function="false" hidden="false" name="Excel_BuiltIn_Sheet_Title_4" vbProcedure="false">"inner"</definedName>
-    <definedName function="false" hidden="false" name="Excel_BuiltIn_Print_Area_5" vbProcedure="false"/>
-    <definedName function="false" hidden="false" name="Excel_BuiltIn_Sheet_Title_5" vbProcedure="false">"interlaced"</definedName>
-    <definedName function="false" hidden="false" name="Excel_BuiltIn_Print_Area_6" vbProcedure="false"/>
-    <definedName function="false" hidden="false" name="Excel_BuiltIn_Sheet_Title_6" vbProcedure="false">"diffs"</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">full!$B$2:$H$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">left!$B$2:$H$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="true">right!$B$2:$H$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="true">inner!$B$2:$H$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="true">interlaced!$B$2:$H$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="true">diffs!$B$2:$H$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="true">append!$B$2:$H$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="true">multicols!$A$1:$I$8</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
@@ -129,449 +122,458 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="72">
-    <font>
-      <name val="Arial"/>
+  <numFmts count="0"/>
+  <fonts count="69">
+    <font>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Sans"/>
-      <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
       <color rgb="D02020"/>
       <u val="none"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
       <color rgb="20D020"/>
       <u val="none"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
       <color rgb="20D020"/>
       <u val="none"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
       <color rgb="20D020"/>
       <u val="none"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
       <color rgb="20D020"/>
       <u val="none"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
       <color rgb="20D020"/>
       <u val="none"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
       <color rgb="20D020"/>
       <u val="none"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
       <color rgb="20D020"/>
       <u val="none"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
       <color rgb="20D020"/>
       <u val="none"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
       <color rgb="20D020"/>
       <u val="none"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
       <color rgb="20D020"/>
       <u val="none"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
       <color rgb="20D020"/>
       <u val="none"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
       <color rgb="20D020"/>
       <u val="none"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
       <color rgb="20D020"/>
       <u val="none"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
       <color rgb="20D020"/>
       <u val="none"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="2020D0"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="2020D0"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
       <color rgb="2020D0"/>
       <u val="none"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="darkGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -579,300 +581,258 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="10" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="11" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="12" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="13" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="14" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="15" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="16" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="17" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="18" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="19" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="20" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="21" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="22" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="23" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="24" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="25" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="26" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="27" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="28" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="29" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="30" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="31" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="32" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="33" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="34" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="35" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="36" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="37" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="38" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="39" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="40" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="41" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="42" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="43" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="44" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="45" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="46" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="47" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="48" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="49" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="50" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="51" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="52" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="53" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="54" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="55" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="56" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="57" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="58" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="59" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="60" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="61" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="62" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="63" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="64" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="65" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="66" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="67" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="68" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="69" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="70" numFmtId="164" xfId="0">
-      <protection/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="71" numFmtId="164" xfId="0">
+  <cellXfs count="69">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="5" borderId="0" xfId="0" applyFont="true" applyFill="true">
       <protection/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-  </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A2:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="10">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="1" width="11.6235294117647" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="1" width="12.6078431372549" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="1" width="11.9019607843137" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="1" width="11.6235294117647" collapsed="true"/>
-    <col min="5" max="5" hidden="false" style="1" width="12.6078431372549" collapsed="true"/>
-    <col min="6" max="6" hidden="false" style="1" width="11.9019607843137" collapsed="true"/>
-    <col min="7" max="256" hidden="false" style="1" width="11.6235294117647" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.01171875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.62890625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.1171875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.9140625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.62890625"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.1171875"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="8.9140625"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="2">
-      <c r="B2" t="s">
+    <row r="2">
+      <c r="B2" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="1">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="1">
         <v>3</v>
       </c>
     </row>
@@ -880,22 +840,22 @@
       <c r="B3" t="n">
         <v>1.0</v>
       </c>
-      <c r="C3" t="s" s="3">
+      <c r="C3" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="D3" t="s" s="3">
+      <c r="D3" t="s" s="2">
         <v>5</v>
       </c>
-      <c r="E3" t="n" s="3">
+      <c r="E3" t="n" s="2">
         <v>11.0</v>
       </c>
-      <c r="F3" t="s" s="3">
+      <c r="F3" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="G3" t="s" s="3">
+      <c r="G3" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="H3" t="n" s="3">
+      <c r="H3" t="n" s="2">
         <v>21.0</v>
       </c>
     </row>
@@ -903,78 +863,78 @@
       <c r="B4" t="n">
         <v>2.0</v>
       </c>
-      <c r="C4" t="s" s="3">
+      <c r="C4" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="D4" t="s" s="3">
+      <c r="D4" t="s" s="2">
         <v>9</v>
       </c>
-      <c r="E4" t="n" s="3">
+      <c r="E4" t="n" s="2">
         <v>12.0</v>
       </c>
-      <c r="F4" t="s" s="3">
+      <c r="F4" t="s" s="2">
         <v>10</v>
       </c>
-      <c r="G4" t="s" s="3">
+      <c r="G4" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="H4" t="n" s="3">
+      <c r="H4" t="n" s="2">
         <v>22.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" t="n" s="3">
+      <c r="B5" t="n" s="2">
         <v>3.0</v>
       </c>
-      <c r="C5" t="s" s="3">
+      <c r="C5" t="s" s="2">
         <v>12</v>
       </c>
-      <c r="D5" t="s" s="3">
+      <c r="D5" t="s" s="2">
         <v>13</v>
       </c>
-      <c r="E5" t="n" s="3">
+      <c r="E5" t="n" s="2">
         <v>13.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" t="n" s="3">
+      <c r="B6" t="n" s="2">
         <v>4.0</v>
       </c>
-      <c r="F6" t="s" s="3">
+      <c r="F6" t="s" s="2">
         <v>14</v>
       </c>
-      <c r="G6" t="s" s="3">
+      <c r="G6" t="s" s="2">
         <v>15</v>
       </c>
-      <c r="H6" t="n" s="3">
+      <c r="H6" t="n" s="2">
         <v>24.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" t="n" s="3">
+      <c r="B7" t="n" s="2">
         <v>5.0</v>
       </c>
-      <c r="C7" t="s" s="3">
+      <c r="C7" t="s" s="2">
         <v>16</v>
       </c>
-      <c r="D7" t="s" s="3">
+      <c r="D7" t="s" s="2">
         <v>17</v>
       </c>
-      <c r="E7" t="n" s="3">
+      <c r="E7" t="n" s="2">
         <v>15.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="B8" t="n" s="3">
+      <c r="B8" t="n" s="2">
         <v>6.0</v>
       </c>
-      <c r="F8" t="s" s="3">
+      <c r="F8" t="s" s="2">
         <v>18</v>
       </c>
-      <c r="G8" t="s" s="3">
+      <c r="G8" t="s" s="2">
         <v>19</v>
       </c>
-      <c r="H8" t="n" s="3">
+      <c r="H8" t="n" s="2">
         <v>26.0</v>
       </c>
     </row>
@@ -1011,7 +971,7 @@
       <c r="D10" t="s">
         <v>23</v>
       </c>
-      <c r="E10" t="n" s="3">
+      <c r="E10" t="n" s="2">
         <v>15.0</v>
       </c>
       <c r="F10" t="s">
@@ -1020,56 +980,53 @@
       <c r="G10" t="s">
         <v>23</v>
       </c>
-      <c r="H10" t="n" s="3">
+      <c r="H10" t="n" s="2">
         <v>88.0</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
+  <autoFilter ref="B2:H10"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="10">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="256" hidden="false" style="1" width="11.6235294117647" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.01171875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.62890625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.1171875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.9140625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.62890625"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.1171875"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="8.9140625"/>
   </cols>
   <sheetData>
     <row r="2">
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="1">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1194,51 +1151,48 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
+  <autoFilter ref="B2:H8"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="10">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="2" width="9.18039215686274" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.01171875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.62890625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.1171875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.9140625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.62890625"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.1171875"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="8.9140625"/>
   </cols>
   <sheetData>
     <row r="2">
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="1">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1363,51 +1317,48 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="1" footer="1"/>
-  <pageSetup blackAndWhite="false" cellComments="atEnd" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;CTAB]</oddHeader>
-    <oddFooter>&amp;CPage PAGE]</oddFooter>
-  </headerFooter>
+  <autoFilter ref="B2:H8"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="10">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="2" width="9.18039215686274" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.01171875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.62890625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.1171875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.9140625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.62890625"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.1171875"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="8.9140625"/>
   </cols>
   <sheetData>
     <row r="2">
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="1">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1504,25 +1455,25 @@
       </c>
     </row>
     <row r="20">
-      <c r="B20" t="s">
+      <c r="B20" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" t="s" s="1">
         <v>3</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" t="s" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1665,51 +1616,48 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="1" footer="1"/>
-  <pageSetup blackAndWhite="false" cellComments="atEnd" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;CTAB]</oddHeader>
-    <oddFooter>&amp;CPage PAGE]</oddFooter>
-  </headerFooter>
+  <autoFilter ref="B20:H26"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="10">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="2" width="9.18039215686274" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.01171875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.62890625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.62890625"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.1171875"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.1171875"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="8.9140625"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="8.9140625"/>
   </cols>
   <sheetData>
     <row r="2">
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="1">
         <v>3</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1862,51 +1810,48 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="1" footer="1"/>
-  <pageSetup blackAndWhite="false" cellComments="atEnd" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;CTAB]</oddHeader>
-    <oddFooter>&amp;CPage PAGE]</oddFooter>
-  </headerFooter>
+  <autoFilter ref="B2:H10"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="10">
-      <selection activeCell="C15" activeCellId="0" pane="topLeft" sqref="C15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="2" width="9.18039215686274" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.01171875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.62890625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.1171875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.9140625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.62890625"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.1171875"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="8.9140625"/>
   </cols>
   <sheetData>
     <row r="2">
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="1">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1914,22 +1859,22 @@
       <c r="B3" t="n">
         <v>1.0</v>
       </c>
-      <c r="C3" t="s" s="3">
+      <c r="C3" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="D3" t="s" s="3">
+      <c r="D3" t="s" s="2">
         <v>5</v>
       </c>
-      <c r="E3" t="n" s="3">
+      <c r="E3" t="n" s="2">
         <v>11.0</v>
       </c>
-      <c r="F3" t="s" s="3">
+      <c r="F3" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="G3" t="s" s="3">
+      <c r="G3" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="H3" t="n" s="3">
+      <c r="H3" t="n" s="2">
         <v>21.0</v>
       </c>
     </row>
@@ -1937,78 +1882,78 @@
       <c r="B4" t="n">
         <v>2.0</v>
       </c>
-      <c r="C4" t="s" s="3">
+      <c r="C4" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="D4" t="s" s="3">
+      <c r="D4" t="s" s="2">
         <v>9</v>
       </c>
-      <c r="E4" t="n" s="3">
+      <c r="E4" t="n" s="2">
         <v>12.0</v>
       </c>
-      <c r="F4" t="s" s="3">
+      <c r="F4" t="s" s="2">
         <v>10</v>
       </c>
-      <c r="G4" t="s" s="3">
+      <c r="G4" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="H4" t="n" s="3">
+      <c r="H4" t="n" s="2">
         <v>22.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" t="n" s="3">
+      <c r="B5" t="n" s="2">
         <v>3.0</v>
       </c>
-      <c r="C5" t="s" s="3">
+      <c r="C5" t="s" s="2">
         <v>12</v>
       </c>
-      <c r="D5" t="s" s="3">
+      <c r="D5" t="s" s="2">
         <v>13</v>
       </c>
-      <c r="E5" t="n" s="3">
+      <c r="E5" t="n" s="2">
         <v>13.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" t="n" s="3">
+      <c r="B6" t="n" s="2">
         <v>4.0</v>
       </c>
-      <c r="F6" t="s" s="3">
+      <c r="F6" t="s" s="2">
         <v>14</v>
       </c>
-      <c r="G6" t="s" s="3">
+      <c r="G6" t="s" s="2">
         <v>15</v>
       </c>
-      <c r="H6" t="n" s="3">
+      <c r="H6" t="n" s="2">
         <v>24.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" t="n" s="3">
+      <c r="B7" t="n" s="2">
         <v>5.0</v>
       </c>
-      <c r="C7" t="s" s="3">
+      <c r="C7" t="s" s="2">
         <v>16</v>
       </c>
-      <c r="D7" t="s" s="3">
+      <c r="D7" t="s" s="2">
         <v>17</v>
       </c>
-      <c r="E7" t="n" s="3">
+      <c r="E7" t="n" s="2">
         <v>15.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="B8" t="n" s="3">
+      <c r="B8" t="n" s="2">
         <v>6.0</v>
       </c>
-      <c r="F8" t="s" s="3">
+      <c r="F8" t="s" s="2">
         <v>18</v>
       </c>
-      <c r="G8" t="s" s="3">
+      <c r="G8" t="s" s="2">
         <v>19</v>
       </c>
-      <c r="H8" t="n" s="3">
+      <c r="H8" t="n" s="2">
         <v>26.0</v>
       </c>
     </row>
@@ -2022,7 +1967,7 @@
       <c r="D9" t="s">
         <v>23</v>
       </c>
-      <c r="E9" t="n" s="3">
+      <c r="E9" t="n" s="2">
         <v>15.0</v>
       </c>
       <c r="F9" t="s">
@@ -2031,18 +1976,13 @@
       <c r="G9" t="s">
         <v>23</v>
       </c>
-      <c r="H9" t="n" s="3">
+      <c r="H9" t="n" s="2">
         <v>88.0</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="atEnd" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <autoFilter ref="B2:H9"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -2053,27 +1993,36 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.01171875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.62890625"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.1171875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.9140625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.62890625"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.1171875"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="8.9140625"/>
+  </cols>
   <sheetData>
     <row r="2">
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="1">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="1">
         <v>3</v>
       </c>
     </row>
@@ -2081,22 +2030,22 @@
       <c r="B3" t="n">
         <v>1.0</v>
       </c>
-      <c r="C3" t="s" s="4">
+      <c r="C3" t="s" s="3">
         <v>4</v>
       </c>
-      <c r="D3" t="s" s="5">
+      <c r="D3" t="s" s="4">
         <v>5</v>
       </c>
-      <c r="E3" t="n" s="6">
+      <c r="E3" t="n" s="5">
         <v>11.0</v>
       </c>
-      <c r="F3" t="s" s="7">
+      <c r="F3" t="s" s="6">
         <v>6</v>
       </c>
-      <c r="G3" t="s" s="8">
+      <c r="G3" t="s" s="7">
         <v>7</v>
       </c>
-      <c r="H3" t="n" s="9">
+      <c r="H3" t="n" s="8">
         <v>21.0</v>
       </c>
     </row>
@@ -2104,22 +2053,22 @@
       <c r="B4" t="n">
         <v>2.0</v>
       </c>
-      <c r="C4" t="s" s="10">
+      <c r="C4" t="s" s="9">
         <v>8</v>
       </c>
-      <c r="D4" t="s" s="11">
+      <c r="D4" t="s" s="10">
         <v>9</v>
       </c>
-      <c r="E4" t="n" s="12">
+      <c r="E4" t="n" s="11">
         <v>12.0</v>
       </c>
-      <c r="F4" t="s" s="13">
+      <c r="F4" t="s" s="12">
         <v>10</v>
       </c>
-      <c r="G4" t="s" s="14">
+      <c r="G4" t="s" s="13">
         <v>11</v>
       </c>
-      <c r="H4" t="n" s="15">
+      <c r="H4" t="n" s="14">
         <v>22.0</v>
       </c>
     </row>
@@ -2133,7 +2082,7 @@
       <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" t="n" s="16">
+      <c r="E5" t="n" s="15">
         <v>15.0</v>
       </c>
       <c r="F5" t="s">
@@ -2142,7 +2091,7 @@
       <c r="G5" t="s">
         <v>23</v>
       </c>
-      <c r="H5" t="n" s="17">
+      <c r="H5" t="n" s="16">
         <v>88.0</v>
       </c>
     </row>
@@ -2150,22 +2099,22 @@
       <c r="B6" t="n">
         <v>1.0</v>
       </c>
-      <c r="C6" t="s" s="18">
+      <c r="C6" t="s" s="17">
         <v>4</v>
       </c>
-      <c r="D6" t="s" s="19">
+      <c r="D6" t="s" s="18">
         <v>5</v>
       </c>
-      <c r="E6" t="n" s="20">
+      <c r="E6" t="n" s="19">
         <v>11.0</v>
       </c>
-      <c r="F6" t="s" s="21">
+      <c r="F6" t="s" s="20">
         <v>6</v>
       </c>
-      <c r="G6" t="s" s="22">
+      <c r="G6" t="s" s="21">
         <v>7</v>
       </c>
-      <c r="H6" t="n" s="23">
+      <c r="H6" t="n" s="22">
         <v>21.0</v>
       </c>
     </row>
@@ -2173,22 +2122,22 @@
       <c r="B7" t="n">
         <v>2.0</v>
       </c>
-      <c r="C7" t="s" s="24">
+      <c r="C7" t="s" s="23">
         <v>8</v>
       </c>
-      <c r="D7" t="s" s="25">
+      <c r="D7" t="s" s="24">
         <v>9</v>
       </c>
-      <c r="E7" t="n" s="26">
+      <c r="E7" t="n" s="25">
         <v>12.0</v>
       </c>
-      <c r="F7" t="s" s="27">
+      <c r="F7" t="s" s="26">
         <v>10</v>
       </c>
-      <c r="G7" t="s" s="28">
+      <c r="G7" t="s" s="27">
         <v>11</v>
       </c>
-      <c r="H7" t="n" s="29">
+      <c r="H7" t="n" s="28">
         <v>22.0</v>
       </c>
     </row>
@@ -2202,7 +2151,7 @@
       <c r="D8" t="s">
         <v>23</v>
       </c>
-      <c r="E8" t="n" s="30">
+      <c r="E8" t="n" s="29">
         <v>15.0</v>
       </c>
       <c r="F8" t="s">
@@ -2211,11 +2160,12 @@
       <c r="G8" t="s">
         <v>23</v>
       </c>
-      <c r="H8" t="n" s="31">
+      <c r="H8" t="n" s="30">
         <v>88.0</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B2:H8"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -2227,33 +2177,44 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.01171875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.2578125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.1484375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.62890625"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.1171875"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.9140625"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.62890625"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="16.1171875"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.9140625"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="1">
         <v>24</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="1">
         <v>25</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="1">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="1">
         <v>3</v>
       </c>
     </row>
@@ -2267,22 +2228,22 @@
       <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" t="s" s="32">
+      <c r="D2" t="s" s="31">
         <v>4</v>
       </c>
-      <c r="E2" t="s" s="33">
+      <c r="E2" t="s" s="32">
         <v>5</v>
       </c>
-      <c r="F2" t="n" s="34">
+      <c r="F2" t="n" s="33">
         <v>11.0</v>
       </c>
-      <c r="G2" t="s" s="35">
+      <c r="G2" t="s" s="34">
         <v>6</v>
       </c>
-      <c r="H2" t="s" s="36">
+      <c r="H2" t="s" s="35">
         <v>7</v>
       </c>
-      <c r="I2" t="n" s="37">
+      <c r="I2" t="n" s="36">
         <v>21.0</v>
       </c>
     </row>
@@ -2296,102 +2257,102 @@
       <c r="C3" t="s">
         <v>27</v>
       </c>
-      <c r="D3" t="s" s="38">
+      <c r="D3" t="s" s="37">
         <v>8</v>
       </c>
-      <c r="E3" t="s" s="39">
+      <c r="E3" t="s" s="38">
         <v>9</v>
       </c>
-      <c r="F3" t="n" s="40">
+      <c r="F3" t="n" s="39">
         <v>12.0</v>
       </c>
-      <c r="G3" t="s" s="41">
+      <c r="G3" t="s" s="40">
         <v>10</v>
       </c>
-      <c r="H3" t="s" s="42">
+      <c r="H3" t="s" s="41">
         <v>11</v>
       </c>
-      <c r="I3" t="n" s="43">
+      <c r="I3" t="n" s="42">
         <v>22.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n" s="44">
+      <c r="A4" t="n" s="43">
         <v>3.0</v>
       </c>
-      <c r="B4" t="s" s="45">
+      <c r="B4" t="s" s="44">
         <v>26</v>
       </c>
-      <c r="C4" t="s" s="46">
+      <c r="C4" t="s" s="45">
         <v>27</v>
       </c>
-      <c r="D4" t="s" s="47">
+      <c r="D4" t="s" s="46">
         <v>12</v>
       </c>
-      <c r="E4" t="s" s="48">
+      <c r="E4" t="s" s="47">
         <v>13</v>
       </c>
-      <c r="F4" t="n" s="49">
+      <c r="F4" t="n" s="48">
         <v>13.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n" s="50">
+      <c r="A5" t="n" s="49">
         <v>4.0</v>
       </c>
-      <c r="B5" t="s" s="51">
+      <c r="B5" t="s" s="50">
         <v>26</v>
       </c>
-      <c r="C5" t="s" s="52">
+      <c r="C5" t="s" s="51">
         <v>28</v>
       </c>
-      <c r="G5" t="s" s="53">
+      <c r="G5" t="s" s="52">
         <v>14</v>
       </c>
-      <c r="H5" t="s" s="54">
+      <c r="H5" t="s" s="53">
         <v>15</v>
       </c>
-      <c r="I5" t="n" s="55">
+      <c r="I5" t="n" s="54">
         <v>24.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n" s="56">
+      <c r="A6" t="n" s="55">
         <v>5.0</v>
       </c>
-      <c r="B6" t="s" s="57">
+      <c r="B6" t="s" s="56">
         <v>26</v>
       </c>
-      <c r="C6" t="s" s="58">
+      <c r="C6" t="s" s="57">
         <v>27</v>
       </c>
-      <c r="D6" t="s" s="59">
+      <c r="D6" t="s" s="58">
         <v>16</v>
       </c>
-      <c r="E6" t="s" s="60">
+      <c r="E6" t="s" s="59">
         <v>17</v>
       </c>
-      <c r="F6" t="n" s="61">
+      <c r="F6" t="n" s="60">
         <v>15.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n" s="62">
+      <c r="A7" t="n" s="61">
         <v>6.0</v>
       </c>
-      <c r="B7" t="s" s="63">
+      <c r="B7" t="s" s="62">
         <v>26</v>
       </c>
-      <c r="C7" t="s" s="64">
+      <c r="C7" t="s" s="63">
         <v>28</v>
       </c>
-      <c r="G7" t="s" s="65">
+      <c r="G7" t="s" s="64">
         <v>18</v>
       </c>
-      <c r="H7" t="s" s="66">
+      <c r="H7" t="s" s="65">
         <v>19</v>
       </c>
-      <c r="I7" t="n" s="67">
+      <c r="I7" t="n" s="66">
         <v>26.0</v>
       </c>
     </row>
@@ -2411,7 +2372,7 @@
       <c r="E8" t="s">
         <v>23</v>
       </c>
-      <c r="F8" t="n" s="68">
+      <c r="F8" t="n" s="67">
         <v>15.0</v>
       </c>
       <c r="G8" t="s">
@@ -2420,11 +2381,12 @@
       <c r="H8" t="s">
         <v>23</v>
       </c>
-      <c r="I8" t="n" s="69">
+      <c r="I8" t="n" s="68">
         <v>88.0</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I8"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
* Added the null ordering auto-detection based on the order obtained from the database. * ADding generated javadoc documentation.
</commit_message>
<xml_diff>
--- a/tests/data/desired/joinreport.xlsx
+++ b/tests/data/desired/joinreport.xlsx
@@ -3268,58 +3268,58 @@
       <c r="A5" t="n" s="105">
         <v>3.0</v>
       </c>
-      <c r="B5" t="s" s="106">
-        <v>33</v>
+      <c r="B5" t="n" s="106">
+        <v>11.0</v>
       </c>
       <c r="C5" t="s" s="107">
         <v>32</v>
       </c>
       <c r="D5" t="s" s="108">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s" s="109">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s" s="110">
-        <v>14</v>
+        <v>35</v>
+      </c>
+      <c r="F5" t="n" s="110">
+        <v>11.0</v>
       </c>
       <c r="G5" t="s" s="111">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="H5" t="s" s="112">
-        <v>35</v>
-      </c>
-      <c r="I5" t="n" s="113">
-        <v>21.0</v>
+        <v>14</v>
+      </c>
+      <c r="I5" t="s" s="113">
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n" s="114">
         <v>3.0</v>
       </c>
-      <c r="B6" t="n" s="115">
-        <v>11.0</v>
+      <c r="B6" t="s" s="115">
+        <v>33</v>
       </c>
       <c r="C6" t="s" s="116">
         <v>32</v>
       </c>
       <c r="D6" t="s" s="117">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s" s="118">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s" s="119">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s" s="120">
         <v>36</v>
       </c>
-      <c r="E6" t="s" s="118">
+      <c r="H6" t="s" s="121">
         <v>35</v>
       </c>
-      <c r="F6" t="n" s="119">
-        <v>11.0</v>
-      </c>
-      <c r="G6" t="s" s="120">
-        <v>14</v>
-      </c>
-      <c r="H6" t="s" s="121">
-        <v>14</v>
-      </c>
-      <c r="I6" t="s" s="122">
-        <v>14</v>
+      <c r="I6" t="n" s="122">
+        <v>21.0</v>
       </c>
     </row>
     <row r="7">
@@ -3388,25 +3388,25 @@
         <v>11.0</v>
       </c>
       <c r="C9" t="s" s="143">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s" s="144">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s" s="145">
-        <v>14</v>
-      </c>
-      <c r="F9" t="s" s="146">
-        <v>14</v>
+        <v>35</v>
+      </c>
+      <c r="F9" t="n" s="146">
+        <v>11.0</v>
       </c>
       <c r="G9" t="s" s="147">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="H9" t="s" s="148">
-        <v>35</v>
-      </c>
-      <c r="I9" t="n" s="149">
-        <v>21.0</v>
+        <v>14</v>
+      </c>
+      <c r="I9" t="s" s="149">
+        <v>14</v>
       </c>
     </row>
     <row r="10">
@@ -3417,25 +3417,25 @@
         <v>11.0</v>
       </c>
       <c r="C10" t="s" s="152">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s" s="153">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s" s="154">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s" s="155">
+        <v>14</v>
+      </c>
+      <c r="G10" t="s" s="156">
         <v>38</v>
       </c>
-      <c r="E10" t="s" s="154">
+      <c r="H10" t="s" s="157">
         <v>35</v>
       </c>
-      <c r="F10" t="n" s="155">
-        <v>11.0</v>
-      </c>
-      <c r="G10" t="s" s="156">
-        <v>14</v>
-      </c>
-      <c r="H10" t="s" s="157">
-        <v>14</v>
-      </c>
-      <c r="I10" t="s" s="158">
-        <v>14</v>
+      <c r="I10" t="n" s="158">
+        <v>21.0</v>
       </c>
     </row>
     <row r="11">

</xml_diff>

<commit_message>
* Finished detailed layout. * Minor code refactoring. * Javadoc newly generated.
</commit_message>
<xml_diff>
--- a/tests/data/desired/joinreport.xlsx
+++ b/tests/data/desired/joinreport.xlsx
@@ -3268,58 +3268,58 @@
       <c r="A5" t="n" s="105">
         <v>3.0</v>
       </c>
-      <c r="B5" t="n" s="106">
-        <v>11.0</v>
+      <c r="B5" t="s" s="106">
+        <v>33</v>
       </c>
       <c r="C5" t="s" s="107">
         <v>32</v>
       </c>
       <c r="D5" t="s" s="108">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s" s="109">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s" s="110">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s" s="111">
         <v>36</v>
       </c>
-      <c r="E5" t="s" s="109">
+      <c r="H5" t="s" s="112">
         <v>35</v>
       </c>
-      <c r="F5" t="n" s="110">
-        <v>11.0</v>
-      </c>
-      <c r="G5" t="s" s="111">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s" s="112">
-        <v>14</v>
-      </c>
-      <c r="I5" t="s" s="113">
-        <v>14</v>
+      <c r="I5" t="n" s="113">
+        <v>21.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n" s="114">
         <v>3.0</v>
       </c>
-      <c r="B6" t="s" s="115">
-        <v>33</v>
+      <c r="B6" t="n" s="115">
+        <v>11.0</v>
       </c>
       <c r="C6" t="s" s="116">
         <v>32</v>
       </c>
       <c r="D6" t="s" s="117">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s" s="118">
-        <v>14</v>
-      </c>
-      <c r="F6" t="s" s="119">
-        <v>14</v>
+        <v>35</v>
+      </c>
+      <c r="F6" t="n" s="119">
+        <v>11.0</v>
       </c>
       <c r="G6" t="s" s="120">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="H6" t="s" s="121">
-        <v>35</v>
-      </c>
-      <c r="I6" t="n" s="122">
-        <v>21.0</v>
+        <v>14</v>
+      </c>
+      <c r="I6" t="s" s="122">
+        <v>14</v>
       </c>
     </row>
     <row r="7">
@@ -3388,25 +3388,25 @@
         <v>11.0</v>
       </c>
       <c r="C9" t="s" s="143">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s" s="144">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s" s="145">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s" s="146">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s" s="147">
         <v>38</v>
       </c>
-      <c r="E9" t="s" s="145">
+      <c r="H9" t="s" s="148">
         <v>35</v>
       </c>
-      <c r="F9" t="n" s="146">
-        <v>11.0</v>
-      </c>
-      <c r="G9" t="s" s="147">
-        <v>14</v>
-      </c>
-      <c r="H9" t="s" s="148">
-        <v>14</v>
-      </c>
-      <c r="I9" t="s" s="149">
-        <v>14</v>
+      <c r="I9" t="n" s="149">
+        <v>21.0</v>
       </c>
     </row>
     <row r="10">
@@ -3417,25 +3417,25 @@
         <v>11.0</v>
       </c>
       <c r="C10" t="s" s="152">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s" s="153">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s" s="154">
-        <v>14</v>
-      </c>
-      <c r="F10" t="s" s="155">
-        <v>14</v>
+        <v>35</v>
+      </c>
+      <c r="F10" t="n" s="155">
+        <v>11.0</v>
       </c>
       <c r="G10" t="s" s="156">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="H10" t="s" s="157">
-        <v>35</v>
-      </c>
-      <c r="I10" t="n" s="158">
-        <v>21.0</v>
+        <v>14</v>
+      </c>
+      <c r="I10" t="s" s="158">
+        <v>14</v>
       </c>
     </row>
     <row r="11">

</xml_diff>

<commit_message>
* Added the test to multiple layouts in one join. * Added the test for complementary join type. * Fixed KeyLayout dump.
</commit_message>
<xml_diff>
--- a/tests/data/desired/joinreport.xlsx
+++ b/tests/data/desired/joinreport.xlsx
@@ -10,28 +10,30 @@
     <sheet name="left" r:id="rId4" sheetId="2"/>
     <sheet name="right" r:id="rId5" sheetId="3"/>
     <sheet name="inner" r:id="rId6" sheetId="4"/>
-    <sheet name="interlaced" r:id="rId7" sheetId="5"/>
-    <sheet name="diffs" r:id="rId8" sheetId="6"/>
-    <sheet name="append" r:id="rId9" sheetId="7"/>
-    <sheet name="multicols" r:id="rId10" sheetId="8"/>
-    <sheet name="multicolsWithNulls" r:id="rId11" sheetId="9"/>
+    <sheet name="complement" r:id="rId7" sheetId="5"/>
+    <sheet name="interlaced" r:id="rId8" sheetId="6"/>
+    <sheet name="diffs" r:id="rId9" sheetId="7"/>
+    <sheet name="append" r:id="rId10" sheetId="8"/>
+    <sheet name="multicols" r:id="rId11" sheetId="9"/>
+    <sheet name="multicolsWithNulls" r:id="rId12" sheetId="10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">full!$B$2:$I$10</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">left!$B$2:$I$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="true">right!$B$2:$I$8</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="true">inner!$B$2:$I$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="true">interlaced!$B$2:$I$10</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="true">diffs!$B$2:$I$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="true">append!$B$2:$I$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="true">multicols!$A$1:$J$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="true">multicolsWithNulls!$A$1:$J$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="true">complement!$A$1:$H$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="true">interlaced!$B$2:$I$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="true">diffs!$B$2:$I$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="true">append!$B$2:$I$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="true">multicols!$A$1:$J$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="true">multicolsWithNulls!$A$1:$J$12</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="45">
   <si>
     <t># of Diffs</t>
   </si>
@@ -1291,7 +1293,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="2" max="2" width="14.03515625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.0" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="26.10546875" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="25.59765625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="18.390625" customWidth="true" bestFit="true"/>
@@ -1536,6 +1538,416 @@
     </row>
   </sheetData>
   <autoFilter ref="B2:I10"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="14.03515625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="7.01171875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="14.0078125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="14.0078125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="26.10546875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="25.59765625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="18.390625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="26.10546875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="25.59765625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="18.390625" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s" s="1">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s" s="1">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s" s="1">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s" s="1">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n" s="82">
+        <v>3.0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s" s="83">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s" s="84">
+        <v>9</v>
+      </c>
+      <c r="G2" t="n" s="85">
+        <v>11.0</v>
+      </c>
+      <c r="H2" t="s" s="86">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s" s="87">
+        <v>11</v>
+      </c>
+      <c r="J2" t="n" s="88">
+        <v>21.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n" s="89">
+        <v>3.0</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s" s="90">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s" s="91">
+        <v>39</v>
+      </c>
+      <c r="G3" t="n" s="92">
+        <v>11.0</v>
+      </c>
+      <c r="H3" t="s" s="93">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s" s="94">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s" s="95">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n" s="96">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s" s="97">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s" s="98">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s" s="99">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s" s="100">
+        <v>38</v>
+      </c>
+      <c r="I4" t="s" s="101">
+        <v>39</v>
+      </c>
+      <c r="J4" t="n" s="102">
+        <v>21.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n" s="103">
+        <v>3.0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s" s="104">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s" s="105">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s" s="106">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s" s="107">
+        <v>40</v>
+      </c>
+      <c r="I5" t="s" s="108">
+        <v>39</v>
+      </c>
+      <c r="J5" t="n" s="109">
+        <v>21.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n" s="110">
+        <v>3.0</v>
+      </c>
+      <c r="B6" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s" s="111">
+        <v>40</v>
+      </c>
+      <c r="F6" t="s" s="112">
+        <v>39</v>
+      </c>
+      <c r="G6" t="n" s="113">
+        <v>11.0</v>
+      </c>
+      <c r="H6" t="s" s="114">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s" s="115">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s" s="116">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n" s="117">
+        <v>3.0</v>
+      </c>
+      <c r="B7" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s" s="118">
+        <v>41</v>
+      </c>
+      <c r="F7" t="s" s="119">
+        <v>39</v>
+      </c>
+      <c r="G7" t="n" s="120">
+        <v>11.0</v>
+      </c>
+      <c r="H7" t="s" s="121">
+        <v>18</v>
+      </c>
+      <c r="I7" t="s" s="122">
+        <v>18</v>
+      </c>
+      <c r="J7" t="s" s="123">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n" s="124">
+        <v>3.0</v>
+      </c>
+      <c r="B8" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s" s="125">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s" s="126">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s" s="127">
+        <v>18</v>
+      </c>
+      <c r="H8" t="s" s="128">
+        <v>41</v>
+      </c>
+      <c r="I8" t="s" s="129">
+        <v>39</v>
+      </c>
+      <c r="J8" t="n" s="130">
+        <v>21.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n" s="131">
+        <v>3.0</v>
+      </c>
+      <c r="B9" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s" s="132">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s" s="133">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s" s="134">
+        <v>18</v>
+      </c>
+      <c r="H9" t="s" s="135">
+        <v>42</v>
+      </c>
+      <c r="I9" t="s" s="136">
+        <v>39</v>
+      </c>
+      <c r="J9" t="n" s="137">
+        <v>21.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n" s="138">
+        <v>3.0</v>
+      </c>
+      <c r="B10" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s" s="139">
+        <v>42</v>
+      </c>
+      <c r="F10" t="s" s="140">
+        <v>39</v>
+      </c>
+      <c r="G10" t="n" s="141">
+        <v>11.0</v>
+      </c>
+      <c r="H10" t="s" s="142">
+        <v>18</v>
+      </c>
+      <c r="I10" t="s" s="143">
+        <v>18</v>
+      </c>
+      <c r="J10" t="s" s="144">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n" s="145">
+        <v>1.0</v>
+      </c>
+      <c r="B11" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" t="n" s="146">
+        <v>11.0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" t="n" s="147">
+        <v>21.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n" s="148">
+        <v>1.0</v>
+      </c>
+      <c r="B12" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" t="n" s="149">
+        <v>11.0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>44</v>
+      </c>
+      <c r="I12" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" t="n" s="150">
+        <v>21.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:J12"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -1549,7 +1961,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="2" max="2" width="14.03515625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.0" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="26.10546875" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="25.59765625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="18.390625" customWidth="true" bestFit="true"/>
@@ -1755,7 +2167,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="2" max="2" width="14.03515625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.0" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="26.10546875" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="25.59765625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="18.390625" customWidth="true" bestFit="true"/>
@@ -1961,7 +2373,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="2" max="2" width="14.03515625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.0" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="26.10546875" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="25.59765625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="18.390625" customWidth="true" bestFit="true"/>
@@ -2296,252 +2708,148 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="2" max="2" width="14.03515625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.0" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="14.03515625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="7.01171875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="26.10546875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="26.10546875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="26.10546875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="25.59765625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="25.59765625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="25.59765625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="18.390625" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="18.390625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="18.390625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s" s="1">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s" s="1">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s" s="1">
+        <v>7</v>
+      </c>
+    </row>
     <row r="2">
-      <c r="B2" t="s" s="1">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s" s="1">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s" s="1">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s" s="1">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s" s="1">
-        <v>6</v>
-      </c>
-      <c r="H2" t="s" s="1">
-        <v>4</v>
-      </c>
-      <c r="I2" t="s" s="1">
-        <v>7</v>
+      <c r="A2" t="n" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="G2" t="n" s="2">
+        <v>13.0</v>
+      </c>
+      <c r="H2" t="s" s="2">
+        <v>18</v>
       </c>
     </row>
     <row r="3">
+      <c r="A3" t="n" s="2">
+        <v>3.0</v>
+      </c>
       <c r="B3" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="I3" t="n">
-        <v>21.0</v>
+        <v>4.0</v>
+      </c>
+      <c r="C3" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="H3" t="n" s="2">
+        <v>24.0</v>
       </c>
     </row>
     <row r="4">
+      <c r="A4" t="n" s="2">
+        <v>3.0</v>
+      </c>
       <c r="B4" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>22.0</v>
+        <v>5.0</v>
+      </c>
+      <c r="C4" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="G4" t="n" s="2">
+        <v>15.0</v>
+      </c>
+      <c r="H4" t="s" s="2">
+        <v>18</v>
       </c>
     </row>
     <row r="5">
+      <c r="A5" t="n" s="2">
+        <v>3.0</v>
+      </c>
       <c r="B5" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="C5" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" t="n">
-        <v>13.0</v>
-      </c>
-      <c r="I5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" t="n">
-        <v>24.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" t="n">
-        <v>15.0</v>
-      </c>
-      <c r="I7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="C8" t="n">
         <v>6.0</v>
       </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="C5" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="F8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="E5" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s" s="2">
         <v>24</v>
       </c>
-      <c r="H8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" t="n">
+      <c r="G5" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="H5" t="n" s="2">
         <v>26.0</v>
       </c>
     </row>
-    <row r="9">
-      <c r="B9" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="C9" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="D9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" t="n">
-        <v>77.0</v>
-      </c>
-      <c r="I9" t="n">
-        <v>77.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="C10" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="D10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" t="n">
-        <v>15.0</v>
-      </c>
-      <c r="I10" t="n">
-        <v>88.0</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="B2:I10"/>
+  <autoFilter ref="A1:H5"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -2555,12 +2863,12 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="2" max="2" width="14.03515625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.0" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="26.10546875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="25.59765625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="18.390625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="26.10546875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="25.59765625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="26.10546875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="25.59765625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="25.59765625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="18.390625" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="18.390625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -2575,205 +2883,231 @@
         <v>2</v>
       </c>
       <c r="E2" t="s" s="1">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s" s="1">
         <v>3</v>
       </c>
-      <c r="F2" t="s" s="1">
+      <c r="G2" t="s" s="1">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s" s="1">
         <v>4</v>
-      </c>
-      <c r="G2" t="s" s="1">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s" s="1">
-        <v>6</v>
       </c>
       <c r="I2" t="s" s="1">
         <v>7</v>
       </c>
     </row>
     <row r="3">
-      <c r="B3" t="n" s="2">
+      <c r="B3" t="n">
         <v>3.0</v>
       </c>
       <c r="C3" t="n">
         <v>1.0</v>
       </c>
-      <c r="D3" t="s" s="2">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s" s="2">
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="n" s="2">
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="n">
         <v>11.0</v>
       </c>
-      <c r="G3" t="s" s="2">
-        <v>10</v>
-      </c>
-      <c r="H3" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="I3" t="n" s="2">
+      <c r="I3" t="n">
         <v>21.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4" t="n" s="2">
+      <c r="B4" t="n">
         <v>3.0</v>
       </c>
       <c r="C4" t="n">
         <v>2.0</v>
       </c>
-      <c r="D4" t="s" s="2">
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s" s="2">
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" t="n" s="2">
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="n">
         <v>12.0</v>
       </c>
-      <c r="G4" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s" s="2">
-        <v>15</v>
-      </c>
-      <c r="I4" t="n" s="2">
+      <c r="I4" t="n">
         <v>22.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" t="n" s="2">
+      <c r="B5" t="n">
         <v>3.0</v>
       </c>
       <c r="C5" t="n">
         <v>3.0</v>
       </c>
-      <c r="D5" t="s" s="2">
+      <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s" s="2">
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
         <v>17</v>
       </c>
-      <c r="F5" t="n" s="2">
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="n">
         <v>13.0</v>
       </c>
-      <c r="G5" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="H5" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="I5" t="s" s="2">
+      <c r="I5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" t="n" s="2">
+      <c r="B6" t="n">
         <v>3.0</v>
       </c>
       <c r="C6" t="n">
         <v>4.0</v>
       </c>
-      <c r="D6" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="F6" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="G6" t="s" s="2">
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="H6" t="s" s="2">
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
         <v>20</v>
       </c>
-      <c r="I6" t="n" s="2">
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" t="n">
         <v>24.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" t="n" s="2">
+      <c r="B7" t="n">
         <v>3.0</v>
       </c>
       <c r="C7" t="n">
         <v>5.0</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="D7" t="s">
         <v>21</v>
       </c>
-      <c r="E7" t="s" s="2">
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
         <v>22</v>
       </c>
-      <c r="F7" t="n" s="2">
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" t="n">
         <v>15.0</v>
       </c>
-      <c r="G7" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="H7" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="I7" t="s" s="2">
+      <c r="I7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8">
-      <c r="B8" t="n" s="2">
+      <c r="B8" t="n">
         <v>3.0</v>
       </c>
       <c r="C8" t="n">
         <v>6.0</v>
       </c>
-      <c r="D8" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="E8" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="F8" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="G8" t="s" s="2">
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
         <v>23</v>
       </c>
-      <c r="H8" t="s" s="2">
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
         <v>24</v>
       </c>
-      <c r="I8" t="n" s="2">
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" t="n">
         <v>26.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="B9" t="n" s="2">
+      <c r="B9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>77.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="n">
         <v>1.0</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C10" t="n">
         <v>8.0</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>27</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" t="s">
         <v>28</v>
       </c>
-      <c r="F9" t="n" s="2">
+      <c r="G10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" t="n">
         <v>15.0</v>
       </c>
-      <c r="G9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" t="n" s="2">
+      <c r="I10" t="n">
         <v>88.0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:I9"/>
+  <autoFilter ref="B2:I10"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -2787,7 +3121,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="2" max="2" width="14.03515625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.0" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="26.10546875" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="25.59765625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="18.390625" customWidth="true" bestFit="true"/>
@@ -2823,163 +3157,189 @@
       </c>
     </row>
     <row r="3">
-      <c r="B3" t="n" s="3">
+      <c r="B3" t="n" s="2">
         <v>3.0</v>
       </c>
       <c r="C3" t="n">
         <v>1.0</v>
       </c>
-      <c r="D3" t="s" s="4">
+      <c r="D3" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="E3" t="s" s="5">
+      <c r="E3" t="s" s="2">
         <v>9</v>
       </c>
-      <c r="F3" t="n" s="6">
+      <c r="F3" t="n" s="2">
         <v>11.0</v>
       </c>
-      <c r="G3" t="s" s="7">
+      <c r="G3" t="s" s="2">
         <v>10</v>
       </c>
-      <c r="H3" t="s" s="8">
+      <c r="H3" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="I3" t="n" s="9">
+      <c r="I3" t="n" s="2">
         <v>21.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4" t="n" s="10">
+      <c r="B4" t="n" s="2">
         <v>3.0</v>
       </c>
       <c r="C4" t="n">
         <v>2.0</v>
       </c>
-      <c r="D4" t="s" s="11">
+      <c r="D4" t="s" s="2">
         <v>12</v>
       </c>
-      <c r="E4" t="s" s="12">
+      <c r="E4" t="s" s="2">
         <v>13</v>
       </c>
-      <c r="F4" t="n" s="13">
+      <c r="F4" t="n" s="2">
         <v>12.0</v>
       </c>
-      <c r="G4" t="s" s="14">
+      <c r="G4" t="s" s="2">
         <v>14</v>
       </c>
-      <c r="H4" t="s" s="15">
+      <c r="H4" t="s" s="2">
         <v>15</v>
       </c>
-      <c r="I4" t="n" s="16">
+      <c r="I4" t="n" s="2">
         <v>22.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" t="n" s="17">
+      <c r="B5" t="n" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D5" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="F5" t="n" s="2">
+        <v>13.0</v>
+      </c>
+      <c r="G5" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="n" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="D6" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="H6" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="I6" t="n" s="2">
+        <v>24.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="n" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="F7" t="n" s="2">
+        <v>15.0</v>
+      </c>
+      <c r="G7" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="H7" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="I7" t="s" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="n" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="D8" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="H8" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="I8" t="n" s="2">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="n" s="2">
         <v>1.0</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C9" t="n">
         <v>8.0</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D9" t="s">
         <v>27</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E9" t="s">
         <v>28</v>
       </c>
-      <c r="F5" t="n" s="18">
+      <c r="F9" t="n" s="2">
         <v>15.0</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G9" t="s">
         <v>27</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H9" t="s">
         <v>28</v>
       </c>
-      <c r="I5" t="n" s="19">
+      <c r="I9" t="n" s="2">
         <v>88.0</v>
       </c>
     </row>
-    <row r="6">
-      <c r="B6" t="n" s="20">
-        <v>3.0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D6" t="s" s="21">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s" s="22">
-        <v>9</v>
-      </c>
-      <c r="F6" t="n" s="23">
-        <v>11.0</v>
-      </c>
-      <c r="G6" t="s" s="24">
-        <v>10</v>
-      </c>
-      <c r="H6" t="s" s="25">
-        <v>11</v>
-      </c>
-      <c r="I6" t="n" s="26">
-        <v>21.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="n" s="27">
-        <v>3.0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="D7" t="s" s="28">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s" s="29">
-        <v>13</v>
-      </c>
-      <c r="F7" t="n" s="30">
-        <v>12.0</v>
-      </c>
-      <c r="G7" t="s" s="31">
-        <v>14</v>
-      </c>
-      <c r="H7" t="s" s="32">
-        <v>15</v>
-      </c>
-      <c r="I7" t="n" s="33">
-        <v>22.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" t="n" s="34">
-        <v>1.0</v>
-      </c>
-      <c r="C8" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="D8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" t="n" s="35">
-        <v>15.0</v>
-      </c>
-      <c r="G8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" t="n" s="36">
-        <v>88.0</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="B2:I8"/>
+  <autoFilter ref="B2:I9"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -2992,8 +3352,214 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
+    <col min="2" max="2" width="14.03515625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="7.01171875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="26.10546875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="25.59765625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="18.390625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="26.10546875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="25.59765625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="18.390625" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="2">
+      <c r="B2" t="s" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s" s="1">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s" s="1">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s" s="1">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="n" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D3" t="s" s="4">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s" s="5">
+        <v>9</v>
+      </c>
+      <c r="F3" t="n" s="6">
+        <v>11.0</v>
+      </c>
+      <c r="G3" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s" s="8">
+        <v>11</v>
+      </c>
+      <c r="I3" t="n" s="9">
+        <v>21.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="n" s="10">
+        <v>3.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D4" t="s" s="11">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s" s="12">
+        <v>13</v>
+      </c>
+      <c r="F4" t="n" s="13">
+        <v>12.0</v>
+      </c>
+      <c r="G4" t="s" s="14">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s" s="15">
+        <v>15</v>
+      </c>
+      <c r="I4" t="n" s="16">
+        <v>22.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="n" s="17">
+        <v>1.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="n" s="18">
+        <v>15.0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" t="n" s="19">
+        <v>88.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="n" s="20">
+        <v>3.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D6" t="s" s="21">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s" s="22">
+        <v>9</v>
+      </c>
+      <c r="F6" t="n" s="23">
+        <v>11.0</v>
+      </c>
+      <c r="G6" t="s" s="24">
+        <v>10</v>
+      </c>
+      <c r="H6" t="s" s="25">
+        <v>11</v>
+      </c>
+      <c r="I6" t="n" s="26">
+        <v>21.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="n" s="27">
+        <v>3.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="D7" t="s" s="28">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s" s="29">
+        <v>13</v>
+      </c>
+      <c r="F7" t="n" s="30">
+        <v>12.0</v>
+      </c>
+      <c r="G7" t="s" s="31">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s" s="32">
+        <v>15</v>
+      </c>
+      <c r="I7" t="n" s="33">
+        <v>22.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="n" s="34">
+        <v>1.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="n" s="35">
+        <v>15.0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" t="n" s="36">
+        <v>88.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B2:I8"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
     <col min="1" max="1" width="14.03515625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="8.0" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="7.01171875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="9.2578125" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="11.1484375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="26.10546875" customWidth="true" bestFit="true"/>
@@ -3264,414 +3830,4 @@
   <autoFilter ref="A1:J8"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="14.03515625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="8.0" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="14.0078125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="14.0078125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="26.10546875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="25.59765625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="18.390625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="26.10546875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="25.59765625" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="18.390625" customWidth="true" bestFit="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s" s="1">
-        <v>34</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>35</v>
-      </c>
-      <c r="E1" t="s" s="1">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s" s="1">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s" s="1">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s" s="1">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s" s="1">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n" s="82">
-        <v>3.0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" t="s" s="83">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s" s="84">
-        <v>9</v>
-      </c>
-      <c r="G2" t="n" s="85">
-        <v>11.0</v>
-      </c>
-      <c r="H2" t="s" s="86">
-        <v>10</v>
-      </c>
-      <c r="I2" t="s" s="87">
-        <v>11</v>
-      </c>
-      <c r="J2" t="n" s="88">
-        <v>21.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n" s="89">
-        <v>3.0</v>
-      </c>
-      <c r="B3" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" t="s" s="90">
-        <v>38</v>
-      </c>
-      <c r="F3" t="s" s="91">
-        <v>39</v>
-      </c>
-      <c r="G3" t="n" s="92">
-        <v>11.0</v>
-      </c>
-      <c r="H3" t="s" s="93">
-        <v>18</v>
-      </c>
-      <c r="I3" t="s" s="94">
-        <v>18</v>
-      </c>
-      <c r="J3" t="s" s="95">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n" s="96">
-        <v>3.0</v>
-      </c>
-      <c r="B4" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" t="s" s="97">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s" s="98">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s" s="99">
-        <v>18</v>
-      </c>
-      <c r="H4" t="s" s="100">
-        <v>38</v>
-      </c>
-      <c r="I4" t="s" s="101">
-        <v>39</v>
-      </c>
-      <c r="J4" t="n" s="102">
-        <v>21.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n" s="103">
-        <v>3.0</v>
-      </c>
-      <c r="B5" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" t="s" s="104">
-        <v>18</v>
-      </c>
-      <c r="F5" t="s" s="105">
-        <v>18</v>
-      </c>
-      <c r="G5" t="s" s="106">
-        <v>18</v>
-      </c>
-      <c r="H5" t="s" s="107">
-        <v>40</v>
-      </c>
-      <c r="I5" t="s" s="108">
-        <v>39</v>
-      </c>
-      <c r="J5" t="n" s="109">
-        <v>21.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n" s="110">
-        <v>3.0</v>
-      </c>
-      <c r="B6" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="D6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" t="s" s="111">
-        <v>40</v>
-      </c>
-      <c r="F6" t="s" s="112">
-        <v>39</v>
-      </c>
-      <c r="G6" t="n" s="113">
-        <v>11.0</v>
-      </c>
-      <c r="H6" t="s" s="114">
-        <v>18</v>
-      </c>
-      <c r="I6" t="s" s="115">
-        <v>18</v>
-      </c>
-      <c r="J6" t="s" s="116">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n" s="117">
-        <v>3.0</v>
-      </c>
-      <c r="B7" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="D7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" t="s" s="118">
-        <v>41</v>
-      </c>
-      <c r="F7" t="s" s="119">
-        <v>39</v>
-      </c>
-      <c r="G7" t="n" s="120">
-        <v>11.0</v>
-      </c>
-      <c r="H7" t="s" s="121">
-        <v>18</v>
-      </c>
-      <c r="I7" t="s" s="122">
-        <v>18</v>
-      </c>
-      <c r="J7" t="s" s="123">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n" s="124">
-        <v>3.0</v>
-      </c>
-      <c r="B8" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="C8" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="D8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" t="s" s="125">
-        <v>18</v>
-      </c>
-      <c r="F8" t="s" s="126">
-        <v>18</v>
-      </c>
-      <c r="G8" t="s" s="127">
-        <v>18</v>
-      </c>
-      <c r="H8" t="s" s="128">
-        <v>41</v>
-      </c>
-      <c r="I8" t="s" s="129">
-        <v>39</v>
-      </c>
-      <c r="J8" t="n" s="130">
-        <v>21.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n" s="131">
-        <v>3.0</v>
-      </c>
-      <c r="B9" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="C9" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="D9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" t="s" s="132">
-        <v>18</v>
-      </c>
-      <c r="F9" t="s" s="133">
-        <v>18</v>
-      </c>
-      <c r="G9" t="s" s="134">
-        <v>18</v>
-      </c>
-      <c r="H9" t="s" s="135">
-        <v>42</v>
-      </c>
-      <c r="I9" t="s" s="136">
-        <v>39</v>
-      </c>
-      <c r="J9" t="n" s="137">
-        <v>21.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n" s="138">
-        <v>3.0</v>
-      </c>
-      <c r="B10" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="C10" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="D10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" t="s" s="139">
-        <v>42</v>
-      </c>
-      <c r="F10" t="s" s="140">
-        <v>39</v>
-      </c>
-      <c r="G10" t="n" s="141">
-        <v>11.0</v>
-      </c>
-      <c r="H10" t="s" s="142">
-        <v>18</v>
-      </c>
-      <c r="I10" t="s" s="143">
-        <v>18</v>
-      </c>
-      <c r="J10" t="s" s="144">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n" s="145">
-        <v>1.0</v>
-      </c>
-      <c r="B11" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="C11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" t="n" s="146">
-        <v>11.0</v>
-      </c>
-      <c r="H11" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" t="s">
-        <v>39</v>
-      </c>
-      <c r="J11" t="n" s="147">
-        <v>21.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n" s="148">
-        <v>1.0</v>
-      </c>
-      <c r="B12" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="C12" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="D12" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" t="n" s="149">
-        <v>11.0</v>
-      </c>
-      <c r="H12" t="s">
-        <v>44</v>
-      </c>
-      <c r="I12" t="s">
-        <v>39</v>
-      </c>
-      <c r="J12" t="n" s="150">
-        <v>21.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:J12"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
 </file>
</xml_diff>